<commit_message>
Resultados iPhone con VGG16
He añadido en la tabla del documento "Resultados INP preprocesadas con class weight" los resultados obtenido al probar con el script de la Issue #31 la red VGG16 con las imágenes de iPhone como test.
</commit_message>
<xml_diff>
--- a/Resultados INP preprocesadas con class weight.xlsx
+++ b/Resultados INP preprocesadas con class weight.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\TFG\Transfer-Learning-EDM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83D2911-8D78-497F-AAF9-60FB39FEB415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA60F2D0-E2DE-47F6-9E98-BAF36DED3C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Baseline</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>iPhone</t>
+  </si>
+  <si>
+    <t>ResNet50V2</t>
+  </si>
+  <si>
+    <t>ResNet101</t>
+  </si>
+  <si>
+    <t>ResNet152</t>
+  </si>
+  <si>
+    <t>InceptionV3</t>
   </si>
 </sst>
 </file>
@@ -75,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -83,15 +95,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,65 +401,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B3" s="1">
+        <v>0.75529999999999997</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.83</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.69</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Script genérico VGG19 / Xception / ResNet50V2 / ResNet101 / ResNet152 (Issue #35)
Nuevas pruebas de otras redes de transfer learning en el script genérico. También he actualizado las métricas en la tabla.
</commit_message>
<xml_diff>
--- a/Resultados INP preprocesadas con class weight.xlsx
+++ b/Resultados INP preprocesadas con class weight.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\TFG\Transfer-Learning-EDM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA60F2D0-E2DE-47F6-9E98-BAF36DED3C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE3C893-EAC9-4BCF-BE19-F39D9DA7E4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,12 +79,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -114,19 +144,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCC"/>
+      <color rgb="FFFF9999"/>
+      <color rgb="FFFF5050"/>
+      <color rgb="FFCCFFFF"/>
+      <color rgb="FF33CCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -404,7 +449,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,58 +459,58 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="7">
         <v>0.75529999999999997</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="7">
         <v>0.76</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="7">
         <v>0.78</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="7">
         <v>0.82</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="7">
         <v>0.83</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="7">
         <v>0.83</v>
       </c>
     </row>
@@ -473,9 +518,15 @@
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="B4" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.53</v>
+      </c>
       <c r="E4" s="1">
         <v>0.71</v>
       </c>
@@ -490,59 +541,119 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="B5" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.72</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="B6" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.53</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="B7" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.53</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="B8" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.64</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="B9" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1"/>

</xml_diff>